<commit_message>
Update code! support multi device running -- Nice!
</commit_message>
<xml_diff>
--- a/page/page_sheet.xlsx
+++ b/page/page_sheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE1811B0-FB60-2C40-BADA-C96EB0248717}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D139AFC4-1E25-824A-AC5A-D927887D5968}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="440" windowWidth="14400" windowHeight="17560" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12480" yWindow="440" windowWidth="14400" windowHeight="17560" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="calendar_page" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="158">
   <si>
     <t>element_name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -626,6 +626,42 @@
   </si>
   <si>
     <t>Screen Recorder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.tcl.fota.system:id/firmware_state_message_idle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>download_version_available</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>new_version</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2BBF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>old_version</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2BBE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>launcher_package</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.tcl.android.launcher</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>expect_update_time</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1011,7 +1047,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="32">
+    <row r="5" spans="1:3" ht="16">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1022,7 +1058,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="32">
+    <row r="6" spans="1:3" ht="16">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -1152,8 +1188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20DB733A-DDE7-C647-9BF1-E17983A628AD}">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="131" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView zoomScale="131" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1514,7 +1550,7 @@
     <col min="3" max="3" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="32">
+    <row r="1" spans="1:3" ht="16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1686,7 +1722,7 @@
     <col min="2" max="3" width="46.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="32">
+    <row r="1" spans="1:3" ht="16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1729,7 +1765,7 @@
     <col min="3" max="3" width="37.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="32">
+    <row r="1" spans="1:3" ht="16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1805,7 +1841,7 @@
     <col min="3" max="3" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="32">
+    <row r="1" spans="1:3" ht="16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1914,7 +1950,7 @@
     <col min="3" max="3" width="28.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="32">
+    <row r="1" spans="1:3" ht="16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1988,10 +2024,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16B290E7-8EBD-6449-B49E-3B9DB0478D19}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView zoomScale="188" workbookViewId="0">
-      <selection sqref="A1:C2"/>
+    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2001,7 +2037,7 @@
     <col min="3" max="3" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="32">
+    <row r="1" spans="1:3" ht="16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2042,6 +2078,61 @@
         <v>64</v>
       </c>
       <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>157</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2066,7 +2157,7 @@
     <col min="3" max="3" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="32">
+    <row r="1" spans="1:3" ht="16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>